<commit_message>
admin update profile and decline leave
</commit_message>
<xml_diff>
--- a/com.OnlineLeaveApplication.framework.SDET37/src/test/resources/OlmEmployeeData1.xlsx
+++ b/com.OnlineLeaveApplication.framework.SDET37/src/test/resources/OlmEmployeeData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\OnlineLeaveApplication\com.OnlineLeaveApplication.framework.SDET37\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68BECFD-F1C5-476B-9343-5FC220EC9E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F838FE-ED1D-4DD2-9190-210D22CEBC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="girigiri" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -741,16 +740,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>1880347</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>188819</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>19</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>216834</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>26894</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -760,7 +759,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA55513-ADA3-040F-57C2-871BCBF4BC9C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1056,8 +1055,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,16 +1871,16 @@
           <controlPr defaultSize="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>18</xdr:col>
+                <xdr:colOff>1876425</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>19</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:colOff>219075</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>

</xml_diff>